<commit_message>
Removal of columns of null values greataer than 40 percent
Removal of columns of null values greataer than 40 percent
</commit_message>
<xml_diff>
--- a/helpers.xlsx
+++ b/helpers.xlsx
@@ -8,17 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Career\Upgrad\CaseStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{A7D051C3-E07B-4BC3-8C1E-47B106CCFEA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A33BBCC8-69F3-46AB-9623-9749C87BC5CC}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{92DF7E96-E991-496D-91FE-46E4BCD79CFB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="4" xr2:uid="{92DF7E96-E991-496D-91FE-46E4BCD79CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
     <sheet name="Sheet3" sheetId="3" r:id="rId3"/>
+    <sheet name="Sheet4" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Z$163</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$B$1:$D$123</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="947" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1268" uniqueCount="392">
   <si>
     <t xml:space="preserve"> 'EMERGENCYSTATE_MODE'</t>
   </si>
@@ -1056,6 +1059,163 @@
   </si>
   <si>
     <t>AMT_REQ_CREDIT_BUREAU_DAY','AMT_REQ_CREDIT_BUREAU_MON','AMT_REQ_CREDIT_BUREAU_QRT','AMT_REQ_CREDIT_BUREAU_WEEK','AMT_REQ_CREDIT_BUREAU_YEAR','EXT_SOURCE_2','EXT_SOURCE_3','HOUR_APPR_PROCESS_START','NAME_TYPE_SUITE','WEEKDAY_APPR_PROCESS_START'</t>
+  </si>
+  <si>
+    <t>'SK_ID_CURR', 'TARGET', 'NAME_CONTRACT_TYPE', 'CODE_GENDER', 'FLAG_OWN_CAR', 'FLAG_OWN_REALTY', 'CNT_CHILDREN', 'AMT_INCOME_TOTAL', 'AMT_CREDIT', 'AMT_ANNUITY', 'AMT_GOODS_PRICE', 'NAME_TYPE_SUITE', 'NAME_INCOME_TYPE', 'NAME_EDUCATION_TYPE', 'NAME_FAMILY_STATUS', 'NAME_HOUSING_TYPE', 'REGION_POPULATION_RELATIVE', 'DAYS_BIRTH', 'DAYS_EMPLOYED', 'DAYS_REGISTRATION', 'DAYS_ID_PUBLISH', 'FLAG_MOBIL', 'FLAG_EMP_PHONE', 'FLAG_WORK_PHONE', 'FLAG_CONT_MOBILE', 'FLAG_PHONE', 'FLAG_EMAIL', 'OCCUPATION_TYPE', 'CNT_FAM_MEMBERS', 'REGION_RATING_CLIENT', 'REGION_RATING_CLIENT_W_CITY', 'WEEKDAY_APPR_PROCESS_START', 'HOUR_APPR_PROCESS_START', 'REG_REGION_NOT_LIVE_REGION', 'REG_REGION_NOT_WORK_REGION', 'LIVE_REGION_NOT_WORK_REGION', 'REG_CITY_NOT_LIVE_CITY', 'REG_CITY_NOT_WORK_CITY', 'LIVE_CITY_NOT_WORK_CITY', 'ORGANIZATION_TYPE', 'EXT_SOURCE_2', 'EXT_SOURCE_3', 'OBS_30_CNT_SOCIAL_CIRCLE', 'DEF_30_CNT_SOCIAL_CIRCLE', 'OBS_60_CNT_SOCIAL_CIRCLE', 'DEF_60_CNT_SOCIAL_CIRCLE',</t>
+  </si>
+  <si>
+    <t>Column Name</t>
+  </si>
+  <si>
+    <t>Null Values Percentage</t>
+  </si>
+  <si>
+    <t>SK_ID_CURR', 'TARGET', 'NAME_CONTRACT_TYPE', 'CODE_GENDER', 'FLAG_OWN_CAR', 'FLAG_OWN_REALTY', 'CNT_CHILDREN', 'AMT_INCOME_TOTAL', 'AMT_CREDIT', 'AMT_ANNUITY', 'AMT_GOODS_PRICE', 'NAME_TYPE_SUITE', 'NAME_INCOME_TYPE', 'NAME_EDUCATION_TYPE', 'NAME_FAMILY_STATUS', 'NAME_HOUSING_TYPE', 'REGION_POPULATION_RELATIVE', 'DAYS_BIRTH', 'DAYS_EMPLOYED', 'DAYS_REGISTRATION', 'DAYS_ID_PUBLISH', 'FLAG_MOBIL', 'FLAG_EMP_PHONE', 'FLAG_WORK_PHONE', 'FLAG_CONT_MOBILE', 'FLAG_PHONE', 'FLAG_EMAIL', 'OCCUPATION_TYPE', 'CNT_FAM_MEMBERS', 'REGION_RATING_CLIENT', 'REGION_RATING_CLIENT_W_CITY', 'WEEKDAY_APPR_PROCESS_START', 'HOUR_APPR_PROCESS_START', 'REG_REGION_NOT_LIVE_REGION', 'REG_REGION_NOT_WORK_REGION', 'LIVE_REGION_NOT_WORK_REGION', 'REG_CITY_NOT_LIVE_CITY', 'REG_CITY_NOT_WORK_CITY', 'LIVE_CITY_NOT_WORK_CITY', 'ORGANIZATION_TYPE', 'EXT_SOURCE_2', 'EXT_SOURCE_3', 'OBS_30_CNT_SOCIAL_CIRCLE', 'DEF_30_CNT_SOCIAL_CIRCLE', 'OBS_60_CNT_SOCIAL_CIRCLE', 'DEF_60_CNT_SOCIAL_CIRCLE',
+       'DAYS_LAST_PHONE_CHANGE', 'FLAG_DOCUMENT_2', 'FLAG_DOCUMENT_3', 'FLAG_DOCUMENT_4', 'FLAG_DOCUMENT_5', 'FLAG_DOCUMENT_6', 'FLAG_DOCUMENT_7', 'FLAG_DOCUMENT_8', 'FLAG_DOCUMENT_9', 'FLAG_DOCUMENT_10', 'FLAG_DOCUMENT_11', 'FLAG_DOCUMENT_12', 'FLAG_DOCUMENT_13', 'FLAG_DOCUMENT_14', 'FLAG_DOCUMENT_15', 'FLAG_DOCUMENT_16', 'FLAG_DOCUMENT_17', 'FLAG_DOCUMENT_18', 'FLAG_DOCUMENT_19', 'FLAG_DOCUMENT_20', 'FLAG_DOCUMENT_21', 'AMT_REQ_CREDIT_BUREAU_HOUR', 'AMT_REQ_CREDIT_BUREAU_DAY', 'AMT_REQ_CREDIT_BUREAU_WEEK', 'AMT_REQ_CREDIT_BUREAU_MON', 'AMT_REQ_CREDIT_BUREAU_QRT', 'AMT_REQ_CREDIT_BUREAU_YEAR'</t>
+  </si>
+  <si>
+    <t>'OWN_CAR_AGE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'EXT_SOURCE_1',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APARTMENTS_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BASEMENTAREA_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BEGINEXPLUATATION_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BUILD_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'COMMONAREA_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ELEVATORS_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ENTRANCES_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMAX_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMIN_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LANDAREA_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAPARTMENTS_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAREA_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAPARTMENTS_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAREA_AVG',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APARTMENTS_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BASEMENTAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BEGINEXPLUATATION_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BUILD_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'COMMONAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ELEVATORS_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ENTRANCES_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMAX_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMIN_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LANDAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAPARTMENTS_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAPARTMENTS_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'APARTMENTS_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'BASEMENTAREA_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BEGINEXPLUATATION_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'YEARS_BUILD_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'COMMONAREA_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ELEVATORS_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'ENTRANCES_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMAX_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FLOORSMIN_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LANDAREA_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAPARTMENTS_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'LIVINGAREA_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAPARTMENTS_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'NONLIVINGAREA_MEDI',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'FONDKAPREMONT_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'HOUSETYPE_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'TOTALAREA_MODE',</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 'WALLSMATERIAL_MODE',</t>
   </si>
 </sst>
 </file>
@@ -1097,7 +1257,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -1107,6 +1267,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -5751,7 +5917,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{46DCBF11-A707-4A02-A51A-09C6D5ED591C}">
   <dimension ref="B5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
@@ -5768,4 +5934,2006 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0D54355C-456E-4518-9C85-9C7273E0466D}">
+  <dimension ref="A1:A3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="65.26953125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" ht="160.5" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A1" s="4" t="s">
+        <v>340</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" ht="259" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="5" t="s">
+        <v>343</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A3" s="1"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4544573D-4321-473B-AD66-F314AA4FEE1C}">
+  <sheetPr filterMode="1"/>
+  <dimension ref="B1:H123"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="3" max="3" width="31.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>341</v>
+      </c>
+      <c r="D1" t="s">
+        <v>342</v>
+      </c>
+      <c r="F1" t="s">
+        <v>79</v>
+      </c>
+      <c r="G1" t="s">
+        <v>79</v>
+      </c>
+      <c r="H1" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B2">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D2">
+        <v>3.9022994299390901E-3</v>
+      </c>
+      <c r="F2" t="s">
+        <v>77</v>
+      </c>
+      <c r="G2" t="s">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>360</v>
+      </c>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B3">
+        <v>8</v>
+      </c>
+      <c r="C3" t="s">
+        <v>77</v>
+      </c>
+      <c r="D3">
+        <v>0</v>
+      </c>
+      <c r="F3" t="s">
+        <v>75</v>
+      </c>
+      <c r="G3" t="s">
+        <v>75</v>
+      </c>
+      <c r="H3" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B4">
+        <v>10</v>
+      </c>
+      <c r="C4" t="s">
+        <v>81</v>
+      </c>
+      <c r="D4">
+        <v>9.0403270126922203E-2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>73</v>
+      </c>
+      <c r="G4" t="s">
+        <v>73</v>
+      </c>
+      <c r="H4" t="s">
+        <v>361</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B5">
+        <v>7</v>
+      </c>
+      <c r="C5" t="s">
+        <v>75</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="F5" t="s">
+        <v>122</v>
+      </c>
+      <c r="G5" t="s">
+        <v>122</v>
+      </c>
+      <c r="H5" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B6">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>258</v>
+      </c>
+      <c r="D6">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F6" t="s">
+        <v>67</v>
+      </c>
+      <c r="G6" t="s">
+        <v>67</v>
+      </c>
+      <c r="H6" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B7">
+        <v>116</v>
+      </c>
+      <c r="C7" t="s">
+        <v>254</v>
+      </c>
+      <c r="D7">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F7" t="s">
+        <v>97</v>
+      </c>
+      <c r="G7" t="s">
+        <v>97</v>
+      </c>
+      <c r="H7" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B8">
+        <v>119</v>
+      </c>
+      <c r="C8" t="s">
+        <v>262</v>
+      </c>
+      <c r="D8">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F8" t="s">
+        <v>100</v>
+      </c>
+      <c r="G8" t="s">
+        <v>100</v>
+      </c>
+      <c r="H8" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B9">
+        <v>120</v>
+      </c>
+      <c r="C9" t="s">
+        <v>264</v>
+      </c>
+      <c r="D9">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F9" t="s">
+        <v>211</v>
+      </c>
+      <c r="G9" t="s">
+        <v>211</v>
+      </c>
+      <c r="H9" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B10">
+        <v>118</v>
+      </c>
+      <c r="C10" t="s">
+        <v>260</v>
+      </c>
+      <c r="D10">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F10" t="s">
+        <v>205</v>
+      </c>
+      <c r="G10" t="s">
+        <v>205</v>
+      </c>
+      <c r="H10" t="s">
+        <v>345</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B11">
+        <v>121</v>
+      </c>
+      <c r="C11" t="s">
+        <v>266</v>
+      </c>
+      <c r="D11">
+        <v>13.501630835969999</v>
+      </c>
+      <c r="F11" t="s">
+        <v>209</v>
+      </c>
+      <c r="G11" t="s">
+        <v>209</v>
+      </c>
+      <c r="H11" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B12">
+        <v>44</v>
+      </c>
+      <c r="C12" t="s">
+        <v>155</v>
+      </c>
+      <c r="D12">
+        <v>50.749729277977004</v>
+      </c>
+      <c r="F12" t="s">
+        <v>81</v>
+      </c>
+      <c r="G12" t="s">
+        <v>81</v>
+      </c>
+      <c r="H12" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B13">
+        <v>72</v>
+      </c>
+      <c r="C13" t="s">
+        <v>184</v>
+      </c>
+      <c r="D13">
+        <v>50.749729277977004</v>
+      </c>
+      <c r="F13" t="s">
+        <v>83</v>
+      </c>
+      <c r="G13" t="s">
+        <v>83</v>
+      </c>
+      <c r="H13" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B14">
+        <v>58</v>
+      </c>
+      <c r="C14" t="s">
+        <v>170</v>
+      </c>
+      <c r="D14">
+        <v>50.749729277977004</v>
+      </c>
+      <c r="F14" t="s">
+        <v>86</v>
+      </c>
+      <c r="G14" t="s">
+        <v>86</v>
+      </c>
+      <c r="H14" t="s">
+        <v>356</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B15">
+        <v>45</v>
+      </c>
+      <c r="C15" t="s">
+        <v>157</v>
+      </c>
+      <c r="D15">
+        <v>58.515955526794102</v>
+      </c>
+      <c r="F15" t="s">
+        <v>88</v>
+      </c>
+      <c r="G15" t="s">
+        <v>88</v>
+      </c>
+      <c r="H15" t="s">
+        <v>357</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B16">
+        <v>73</v>
+      </c>
+      <c r="C16" t="s">
+        <v>185</v>
+      </c>
+      <c r="D16">
+        <v>58.515955526794102</v>
+      </c>
+      <c r="F16" t="s">
+        <v>90</v>
+      </c>
+      <c r="G16" t="s">
+        <v>90</v>
+      </c>
+      <c r="H16" t="s">
+        <v>358</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B17">
+        <v>59</v>
+      </c>
+      <c r="C17" t="s">
+        <v>171</v>
+      </c>
+      <c r="D17">
+        <v>58.515955526794102</v>
+      </c>
+      <c r="F17" t="s">
+        <v>92</v>
+      </c>
+      <c r="G17" t="s">
+        <v>92</v>
+      </c>
+      <c r="H17" t="s">
+        <v>359</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B18">
+        <v>6</v>
+      </c>
+      <c r="C18" t="s">
+        <v>73</v>
+      </c>
+      <c r="D18">
+        <v>0</v>
+      </c>
+      <c r="F18" t="s">
+        <v>151</v>
+      </c>
+      <c r="G18" t="s">
+        <v>151</v>
+      </c>
+      <c r="H18" t="s">
+        <v>381</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B19">
+        <v>29</v>
+      </c>
+      <c r="C19" t="s">
+        <v>122</v>
+      </c>
+      <c r="D19">
+        <v>6.5038323832318197E-4</v>
+      </c>
+      <c r="F19" t="s">
+        <v>154</v>
+      </c>
+      <c r="G19" t="s">
+        <v>154</v>
+      </c>
+      <c r="H19" t="s">
+        <v>367</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B20">
+        <v>3</v>
+      </c>
+      <c r="C20" t="s">
+        <v>67</v>
+      </c>
+      <c r="D20">
+        <v>0</v>
+      </c>
+      <c r="F20" t="s">
+        <v>115</v>
+      </c>
+      <c r="G20" t="s">
+        <v>115</v>
+      </c>
+      <c r="H20" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B21">
+        <v>48</v>
+      </c>
+      <c r="C21" t="s">
+        <v>160</v>
+      </c>
+      <c r="D21">
+        <v>69.872297251155203</v>
+      </c>
+      <c r="F21" t="s">
+        <v>102</v>
+      </c>
+      <c r="G21" t="s">
+        <v>102</v>
+      </c>
+      <c r="H21" t="s">
+        <v>363</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B22">
+        <v>76</v>
+      </c>
+      <c r="C22" t="s">
+        <v>188</v>
+      </c>
+      <c r="D22">
+        <v>69.872297251155203</v>
+      </c>
+      <c r="F22" t="s">
+        <v>104</v>
+      </c>
+      <c r="G22" t="s">
+        <v>104</v>
+      </c>
+      <c r="H22" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B23">
+        <v>62</v>
+      </c>
+      <c r="C23" t="s">
+        <v>174</v>
+      </c>
+      <c r="D23">
+        <v>69.872297251155203</v>
+      </c>
+      <c r="F23" t="s">
+        <v>108</v>
+      </c>
+      <c r="G23" t="s">
+        <v>108</v>
+      </c>
+      <c r="H23" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B24">
+        <v>17</v>
+      </c>
+      <c r="C24" t="s">
+        <v>97</v>
+      </c>
+      <c r="D24">
+        <v>0</v>
+      </c>
+      <c r="F24" t="s">
+        <v>230</v>
+      </c>
+      <c r="G24" t="s">
+        <v>230</v>
+      </c>
+      <c r="H24" t="s">
+        <v>368</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B25">
+        <v>18</v>
+      </c>
+      <c r="C25" t="s">
+        <v>100</v>
+      </c>
+      <c r="D25">
+        <v>0</v>
+      </c>
+      <c r="F25" t="s">
+        <v>232</v>
+      </c>
+      <c r="G25" t="s">
+        <v>232</v>
+      </c>
+      <c r="H25" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B26">
+        <v>20</v>
+      </c>
+      <c r="C26" t="s">
+        <v>104</v>
+      </c>
+      <c r="D26">
+        <v>0</v>
+      </c>
+      <c r="F26" t="s">
+        <v>234</v>
+      </c>
+      <c r="G26" t="s">
+        <v>234</v>
+      </c>
+      <c r="H26" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B27">
+        <v>95</v>
+      </c>
+      <c r="C27" t="s">
+        <v>211</v>
+      </c>
+      <c r="D27">
+        <v>3.2519161916159099E-4</v>
+      </c>
+      <c r="F27" t="s">
+        <v>236</v>
+      </c>
+      <c r="G27" t="s">
+        <v>236</v>
+      </c>
+      <c r="H27" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B28">
+        <v>19</v>
+      </c>
+      <c r="C28" t="s">
+        <v>102</v>
+      </c>
+      <c r="D28">
+        <v>0</v>
+      </c>
+      <c r="F28" t="s">
+        <v>238</v>
+      </c>
+      <c r="G28" t="s">
+        <v>238</v>
+      </c>
+      <c r="H28" t="s">
+        <v>369</v>
+      </c>
+    </row>
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B29">
+        <v>92</v>
+      </c>
+      <c r="C29" t="s">
+        <v>205</v>
+      </c>
+      <c r="D29">
+        <v>0.332020643163984</v>
+      </c>
+      <c r="F29" t="s">
+        <v>240</v>
+      </c>
+      <c r="G29" t="s">
+        <v>240</v>
+      </c>
+      <c r="H29" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B30">
+        <v>94</v>
+      </c>
+      <c r="C30" t="s">
+        <v>209</v>
+      </c>
+      <c r="D30">
+        <v>0.332020643163984</v>
+      </c>
+      <c r="F30" t="s">
+        <v>242</v>
+      </c>
+      <c r="G30" t="s">
+        <v>242</v>
+      </c>
+      <c r="H30" t="s">
+        <v>370</v>
+      </c>
+    </row>
+    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B31">
+        <v>49</v>
+      </c>
+      <c r="C31" t="s">
+        <v>161</v>
+      </c>
+      <c r="D31">
+        <v>53.2959796560123</v>
+      </c>
+      <c r="F31" t="s">
+        <v>124</v>
+      </c>
+      <c r="G31" t="s">
+        <v>124</v>
+      </c>
+      <c r="H31" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B32">
+        <v>77</v>
+      </c>
+      <c r="C32" t="s">
+        <v>189</v>
+      </c>
+      <c r="D32">
+        <v>53.2959796560123</v>
+      </c>
+      <c r="F32" t="s">
+        <v>126</v>
+      </c>
+      <c r="G32" t="s">
+        <v>126</v>
+      </c>
+      <c r="H32" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B33">
+        <v>63</v>
+      </c>
+      <c r="C33" t="s">
+        <v>175</v>
+      </c>
+      <c r="D33">
+        <v>53.2959796560123</v>
+      </c>
+      <c r="F33" t="s">
+        <v>128</v>
+      </c>
+      <c r="G33" t="s">
+        <v>128</v>
+      </c>
+      <c r="H33" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B34">
+        <v>90</v>
+      </c>
+      <c r="C34" t="s">
+        <v>202</v>
+      </c>
+      <c r="D34">
+        <v>47.398304450897598</v>
+      </c>
+      <c r="F34" t="s">
+        <v>130</v>
+      </c>
+      <c r="G34" t="s">
+        <v>130</v>
+      </c>
+      <c r="H34" t="s">
+        <v>376</v>
+      </c>
+    </row>
+    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B35">
+        <v>50</v>
+      </c>
+      <c r="C35" t="s">
+        <v>162</v>
+      </c>
+      <c r="D35">
+        <v>50.348768011550803</v>
+      </c>
+      <c r="F35" t="s">
+        <v>133</v>
+      </c>
+      <c r="G35" t="s">
+        <v>133</v>
+      </c>
+      <c r="H35" t="s">
+        <v>377</v>
+      </c>
+    </row>
+    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B36">
+        <v>78</v>
+      </c>
+      <c r="C36" t="s">
+        <v>190</v>
+      </c>
+      <c r="D36">
+        <v>50.348768011550803</v>
+      </c>
+      <c r="F36" t="s">
+        <v>135</v>
+      </c>
+      <c r="G36" t="s">
+        <v>135</v>
+      </c>
+      <c r="H36" t="s">
+        <v>378</v>
+      </c>
+    </row>
+    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B37">
+        <v>64</v>
+      </c>
+      <c r="C37" t="s">
+        <v>176</v>
+      </c>
+      <c r="D37">
+        <v>50.348768011550803</v>
+      </c>
+      <c r="F37" t="s">
+        <v>137</v>
+      </c>
+      <c r="G37" t="s">
+        <v>137</v>
+      </c>
+      <c r="H37" t="s">
+        <v>379</v>
+      </c>
+    </row>
+    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B38">
+        <v>41</v>
+      </c>
+      <c r="C38" t="s">
+        <v>147</v>
+      </c>
+      <c r="D38">
+        <v>56.381072546998297</v>
+      </c>
+      <c r="F38" t="s">
+        <v>139</v>
+      </c>
+      <c r="G38" t="s">
+        <v>139</v>
+      </c>
+      <c r="H38" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B39">
+        <v>42</v>
+      </c>
+      <c r="C39" t="s">
+        <v>151</v>
+      </c>
+      <c r="D39">
+        <v>0.21462646864665</v>
+      </c>
+      <c r="F39" t="s">
+        <v>244</v>
+      </c>
+      <c r="G39" t="s">
+        <v>244</v>
+      </c>
+      <c r="H39" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B40">
+        <v>43</v>
+      </c>
+      <c r="C40" t="s">
+        <v>154</v>
+      </c>
+      <c r="D40">
+        <v>19.825307062186301</v>
+      </c>
+      <c r="F40" t="s">
+        <v>246</v>
+      </c>
+      <c r="G40" t="s">
+        <v>246</v>
+      </c>
+      <c r="H40" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B41">
+        <v>25</v>
+      </c>
+      <c r="C41" t="s">
+        <v>115</v>
+      </c>
+      <c r="D41">
+        <v>0</v>
+      </c>
+      <c r="F41" t="s">
+        <v>248</v>
+      </c>
+      <c r="G41" t="s">
+        <v>248</v>
+      </c>
+      <c r="H41" t="s">
+        <v>386</v>
+      </c>
+    </row>
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B42">
+        <v>104</v>
+      </c>
+      <c r="C42" t="s">
+        <v>230</v>
+      </c>
+      <c r="D42">
+        <v>0</v>
+      </c>
+      <c r="F42" t="s">
+        <v>214</v>
+      </c>
+      <c r="G42" t="s">
+        <v>214</v>
+      </c>
+      <c r="H42" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B43">
+        <v>105</v>
+      </c>
+      <c r="C43" t="s">
+        <v>232</v>
+      </c>
+      <c r="D43">
+        <v>0</v>
+      </c>
+      <c r="F43" t="s">
+        <v>250</v>
+      </c>
+      <c r="G43" t="s">
+        <v>250</v>
+      </c>
+      <c r="H43" t="s">
+        <v>387</v>
+      </c>
+    </row>
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B44">
+        <v>106</v>
+      </c>
+      <c r="C44" t="s">
+        <v>234</v>
+      </c>
+      <c r="D44">
+        <v>0</v>
+      </c>
+      <c r="F44" t="s">
+        <v>252</v>
+      </c>
+      <c r="G44" t="s">
+        <v>252</v>
+      </c>
+      <c r="H44" t="s">
+        <v>390</v>
+      </c>
+    </row>
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B45">
+        <v>107</v>
+      </c>
+      <c r="C45" t="s">
+        <v>236</v>
+      </c>
+      <c r="D45">
+        <v>0</v>
+      </c>
+      <c r="F45" t="s">
+        <v>216</v>
+      </c>
+      <c r="G45" t="s">
+        <v>216</v>
+      </c>
+      <c r="H45" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B46">
+        <v>108</v>
+      </c>
+      <c r="C46" t="s">
+        <v>238</v>
+      </c>
+      <c r="D46">
+        <v>0</v>
+      </c>
+      <c r="F46" t="s">
+        <v>218</v>
+      </c>
+      <c r="G46" t="s">
+        <v>218</v>
+      </c>
+      <c r="H46" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B47">
+        <v>109</v>
+      </c>
+      <c r="C47" t="s">
+        <v>240</v>
+      </c>
+      <c r="D47">
+        <v>0</v>
+      </c>
+      <c r="F47" t="s">
+        <v>220</v>
+      </c>
+      <c r="G47" t="s">
+        <v>220</v>
+      </c>
+      <c r="H47" t="s">
+        <v>362</v>
+      </c>
+    </row>
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B48">
+        <v>110</v>
+      </c>
+      <c r="C48" t="s">
+        <v>242</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="F48" t="s">
+        <v>222</v>
+      </c>
+      <c r="G48" t="s">
+        <v>222</v>
+      </c>
+      <c r="H48" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B49">
+        <v>111</v>
+      </c>
+      <c r="C49" t="s">
+        <v>244</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="F49" t="s">
+        <v>224</v>
+      </c>
+      <c r="G49" t="s">
+        <v>224</v>
+      </c>
+      <c r="H49" t="s">
+        <v>344</v>
+      </c>
+    </row>
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B50">
+        <v>112</v>
+      </c>
+      <c r="C50" t="s">
+        <v>246</v>
+      </c>
+      <c r="D50">
+        <v>0</v>
+      </c>
+      <c r="F50" t="s">
+        <v>226</v>
+      </c>
+      <c r="G50" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B51">
+        <v>113</v>
+      </c>
+      <c r="C51" t="s">
+        <v>248</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="F51" t="s">
+        <v>228</v>
+      </c>
+      <c r="G51" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B52">
+        <v>96</v>
+      </c>
+      <c r="C52" t="s">
+        <v>214</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="F52" t="s">
+        <v>118</v>
+      </c>
+      <c r="G52" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B53">
+        <v>114</v>
+      </c>
+      <c r="C53" t="s">
+        <v>250</v>
+      </c>
+      <c r="D53">
+        <v>0</v>
+      </c>
+      <c r="F53" t="s">
+        <v>111</v>
+      </c>
+      <c r="G53" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B54">
+        <v>115</v>
+      </c>
+      <c r="C54" t="s">
+        <v>252</v>
+      </c>
+      <c r="D54">
+        <v>0</v>
+      </c>
+      <c r="F54" t="s">
+        <v>69</v>
+      </c>
+      <c r="G54" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B55">
+        <v>97</v>
+      </c>
+      <c r="C55" t="s">
+        <v>216</v>
+      </c>
+      <c r="D55">
+        <v>0</v>
+      </c>
+      <c r="F55" t="s">
+        <v>71</v>
+      </c>
+      <c r="G55" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B56">
+        <v>98</v>
+      </c>
+      <c r="C56" t="s">
+        <v>218</v>
+      </c>
+      <c r="D56">
+        <v>0</v>
+      </c>
+      <c r="F56" t="s">
+        <v>117</v>
+      </c>
+      <c r="G56" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B57">
+        <v>99</v>
+      </c>
+      <c r="C57" t="s">
+        <v>220</v>
+      </c>
+      <c r="D57">
+        <v>0</v>
+      </c>
+      <c r="F57" t="s">
+        <v>113</v>
+      </c>
+      <c r="G57" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B58">
+        <v>100</v>
+      </c>
+      <c r="C58" t="s">
+        <v>222</v>
+      </c>
+      <c r="D58">
+        <v>0</v>
+      </c>
+      <c r="F58" t="s">
+        <v>143</v>
+      </c>
+      <c r="G58" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B59">
+        <v>101</v>
+      </c>
+      <c r="C59" t="s">
+        <v>224</v>
+      </c>
+      <c r="D59">
+        <v>0</v>
+      </c>
+      <c r="F59" t="s">
+        <v>65</v>
+      </c>
+      <c r="G59" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B60">
+        <v>102</v>
+      </c>
+      <c r="C60" t="s">
+        <v>226</v>
+      </c>
+      <c r="D60">
+        <v>0</v>
+      </c>
+      <c r="F60" t="s">
+        <v>203</v>
+      </c>
+      <c r="G60" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B61">
+        <v>103</v>
+      </c>
+      <c r="C61" t="s">
+        <v>228</v>
+      </c>
+      <c r="D61">
+        <v>0</v>
+      </c>
+      <c r="F61" t="s">
+        <v>207</v>
+      </c>
+      <c r="G61" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B62">
+        <v>27</v>
+      </c>
+      <c r="C62" t="s">
+        <v>118</v>
+      </c>
+      <c r="D62">
+        <v>0</v>
+      </c>
+      <c r="F62" t="s">
+        <v>120</v>
+      </c>
+      <c r="G62" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B63">
+        <v>23</v>
+      </c>
+      <c r="C63" t="s">
+        <v>111</v>
+      </c>
+      <c r="D63">
+        <v>0</v>
+      </c>
+      <c r="F63" t="s">
+        <v>145</v>
+      </c>
+      <c r="G63" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
+      <c r="B64">
+        <v>22</v>
+      </c>
+      <c r="C64" t="s">
+        <v>108</v>
+      </c>
+      <c r="D64">
+        <v>0</v>
+      </c>
+      <c r="F64" t="s">
+        <v>141</v>
+      </c>
+      <c r="G64" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B65">
+        <v>4</v>
+      </c>
+      <c r="C65" t="s">
+        <v>69</v>
+      </c>
+      <c r="D65">
+        <v>0</v>
+      </c>
+      <c r="F65" t="s">
+        <v>94</v>
+      </c>
+      <c r="G65" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B66">
+        <v>5</v>
+      </c>
+      <c r="C66" t="s">
+        <v>71</v>
+      </c>
+      <c r="D66">
+        <v>0</v>
+      </c>
+      <c r="F66" t="s">
+        <v>58</v>
+      </c>
+      <c r="G66" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B67">
+        <v>26</v>
+      </c>
+      <c r="C67" t="s">
+        <v>117</v>
+      </c>
+      <c r="D67">
+        <v>0</v>
+      </c>
+      <c r="F67" t="s">
+        <v>63</v>
+      </c>
+      <c r="G67" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B68">
+        <v>24</v>
+      </c>
+      <c r="C68" t="s">
+        <v>113</v>
+      </c>
+      <c r="D68">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="69" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B69">
+        <v>51</v>
+      </c>
+      <c r="C69" t="s">
+        <v>163</v>
+      </c>
+      <c r="D69">
+        <v>49.7608215641066</v>
+      </c>
+      <c r="F69" t="s">
+        <v>254</v>
+      </c>
+      <c r="G69" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B70">
+        <v>79</v>
+      </c>
+      <c r="C70" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70">
+        <v>49.7608215641066</v>
+      </c>
+      <c r="F70" t="s">
+        <v>258</v>
+      </c>
+      <c r="G70" t="s">
+        <v>258</v>
+      </c>
+    </row>
+    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B71">
+        <v>65</v>
+      </c>
+      <c r="C71" t="s">
+        <v>177</v>
+      </c>
+      <c r="D71">
+        <v>49.7608215641066</v>
+      </c>
+      <c r="F71" t="s">
+        <v>260</v>
+      </c>
+      <c r="G71" t="s">
+        <v>260</v>
+      </c>
+    </row>
+    <row r="72" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B72">
+        <v>52</v>
+      </c>
+      <c r="C72" t="s">
+        <v>164</v>
+      </c>
+      <c r="D72">
+        <v>67.848629805112594</v>
+      </c>
+      <c r="F72" t="s">
+        <v>262</v>
+      </c>
+      <c r="G72" t="s">
+        <v>262</v>
+      </c>
+    </row>
+    <row r="73" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B73">
+        <v>80</v>
+      </c>
+      <c r="C73" t="s">
+        <v>192</v>
+      </c>
+      <c r="D73">
+        <v>67.848629805112594</v>
+      </c>
+      <c r="F73" t="s">
+        <v>264</v>
+      </c>
+      <c r="G73" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="74" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B74">
+        <v>66</v>
+      </c>
+      <c r="C74" t="s">
+        <v>178</v>
+      </c>
+      <c r="D74">
+        <v>67.848629805112594</v>
+      </c>
+      <c r="F74" t="s">
+        <v>266</v>
+      </c>
+      <c r="G74" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="75" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B75">
+        <v>86</v>
+      </c>
+      <c r="C75" t="s">
+        <v>198</v>
+      </c>
+      <c r="D75">
+        <v>68.386171551586699</v>
+      </c>
+    </row>
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
+      <c r="B76">
+        <v>33</v>
+      </c>
+      <c r="C76" t="s">
+        <v>130</v>
+      </c>
+      <c r="D76">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="77" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B77">
+        <v>87</v>
+      </c>
+      <c r="C77" t="s">
+        <v>199</v>
+      </c>
+      <c r="D77">
+        <v>50.176091261776001</v>
+      </c>
+    </row>
+    <row r="78" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B78">
+        <v>53</v>
+      </c>
+      <c r="C78" t="s">
+        <v>165</v>
+      </c>
+      <c r="D78">
+        <v>59.376737742714802</v>
+      </c>
+    </row>
+    <row r="79" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B79">
+        <v>81</v>
+      </c>
+      <c r="C79" t="s">
+        <v>193</v>
+      </c>
+      <c r="D79">
+        <v>59.376737742714802</v>
+      </c>
+    </row>
+    <row r="80" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B80">
+        <v>67</v>
+      </c>
+      <c r="C80" t="s">
+        <v>179</v>
+      </c>
+      <c r="D80">
+        <v>59.376737742714802</v>
+      </c>
+    </row>
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B81">
+        <v>39</v>
+      </c>
+      <c r="C81" t="s">
+        <v>143</v>
+      </c>
+      <c r="D81">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B82">
+        <v>36</v>
+      </c>
+      <c r="C82" t="s">
+        <v>137</v>
+      </c>
+      <c r="D82">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="83" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B83">
+        <v>54</v>
+      </c>
+      <c r="C83" t="s">
+        <v>166</v>
+      </c>
+      <c r="D83">
+        <v>68.354953156147204</v>
+      </c>
+    </row>
+    <row r="84" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B84">
+        <v>82</v>
+      </c>
+      <c r="C84" t="s">
+        <v>194</v>
+      </c>
+      <c r="D84">
+        <v>68.354953156147204</v>
+      </c>
+    </row>
+    <row r="85" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B85">
+        <v>68</v>
+      </c>
+      <c r="C85" t="s">
+        <v>180</v>
+      </c>
+      <c r="D85">
+        <v>68.354953156147204</v>
+      </c>
+    </row>
+    <row r="86" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B86">
+        <v>55</v>
+      </c>
+      <c r="C86" t="s">
+        <v>167</v>
+      </c>
+      <c r="D86">
+        <v>50.1933264175915</v>
+      </c>
+    </row>
+    <row r="87" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B87">
+        <v>83</v>
+      </c>
+      <c r="C87" t="s">
+        <v>195</v>
+      </c>
+      <c r="D87">
+        <v>50.1933264175915</v>
+      </c>
+    </row>
+    <row r="88" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B88">
+        <v>69</v>
+      </c>
+      <c r="C88" t="s">
+        <v>181</v>
+      </c>
+      <c r="D88">
+        <v>50.1933264175915</v>
+      </c>
+    </row>
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B89">
+        <v>2</v>
+      </c>
+      <c r="C89" t="s">
+        <v>65</v>
+      </c>
+      <c r="D89">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B90">
+        <v>13</v>
+      </c>
+      <c r="C90" t="s">
+        <v>88</v>
+      </c>
+      <c r="D90">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B91">
+        <v>14</v>
+      </c>
+      <c r="C91" t="s">
+        <v>90</v>
+      </c>
+      <c r="D91">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B92">
+        <v>15</v>
+      </c>
+      <c r="C92" t="s">
+        <v>92</v>
+      </c>
+      <c r="D92">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B93">
+        <v>12</v>
+      </c>
+      <c r="C93" t="s">
+        <v>86</v>
+      </c>
+      <c r="D93">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B94">
+        <v>11</v>
+      </c>
+      <c r="C94" t="s">
+        <v>83</v>
+      </c>
+      <c r="D94">
+        <v>0.42014757195677499</v>
+      </c>
+    </row>
+    <row r="95" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B95">
+        <v>56</v>
+      </c>
+      <c r="C95" t="s">
+        <v>168</v>
+      </c>
+      <c r="D95">
+        <v>69.432963373667903</v>
+      </c>
+    </row>
+    <row r="96" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B96">
+        <v>84</v>
+      </c>
+      <c r="C96" t="s">
+        <v>196</v>
+      </c>
+      <c r="D96">
+        <v>69.432963373667903</v>
+      </c>
+    </row>
+    <row r="97" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B97">
+        <v>70</v>
+      </c>
+      <c r="C97" t="s">
+        <v>182</v>
+      </c>
+      <c r="D97">
+        <v>69.432963373667903</v>
+      </c>
+    </row>
+    <row r="98" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B98">
+        <v>57</v>
+      </c>
+      <c r="C98" t="s">
+        <v>169</v>
+      </c>
+      <c r="D98">
+        <v>55.179164322577002</v>
+      </c>
+    </row>
+    <row r="99" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B99">
+        <v>85</v>
+      </c>
+      <c r="C99" t="s">
+        <v>197</v>
+      </c>
+      <c r="D99">
+        <v>55.179164322577002</v>
+      </c>
+    </row>
+    <row r="100" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B100">
+        <v>71</v>
+      </c>
+      <c r="C100" t="s">
+        <v>183</v>
+      </c>
+      <c r="D100">
+        <v>55.179164322577002</v>
+      </c>
+    </row>
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B101">
+        <v>91</v>
+      </c>
+      <c r="C101" t="s">
+        <v>203</v>
+      </c>
+      <c r="D101">
+        <v>0.332020643163984</v>
+      </c>
+    </row>
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B102">
+        <v>93</v>
+      </c>
+      <c r="C102" t="s">
+        <v>207</v>
+      </c>
+      <c r="D102">
+        <v>0.332020643163984</v>
+      </c>
+    </row>
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B103">
+        <v>28</v>
+      </c>
+      <c r="C103" t="s">
+        <v>120</v>
+      </c>
+      <c r="D103">
+        <v>31.345545362604899</v>
+      </c>
+    </row>
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B104">
+        <v>40</v>
+      </c>
+      <c r="C104" t="s">
+        <v>145</v>
+      </c>
+      <c r="D104">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="105" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B105">
+        <v>21</v>
+      </c>
+      <c r="C105" t="s">
+        <v>106</v>
+      </c>
+      <c r="D105">
+        <v>65.990810084842494</v>
+      </c>
+    </row>
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B106">
+        <v>37</v>
+      </c>
+      <c r="C106" t="s">
+        <v>139</v>
+      </c>
+      <c r="D106">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B107">
+        <v>38</v>
+      </c>
+      <c r="C107" t="s">
+        <v>141</v>
+      </c>
+      <c r="D107">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B108">
+        <v>34</v>
+      </c>
+      <c r="C108" t="s">
+        <v>133</v>
+      </c>
+      <c r="D108">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B109">
+        <v>35</v>
+      </c>
+      <c r="C109" t="s">
+        <v>135</v>
+      </c>
+      <c r="D109">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B110">
+        <v>16</v>
+      </c>
+      <c r="C110" t="s">
+        <v>94</v>
+      </c>
+      <c r="D110">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B111">
+        <v>30</v>
+      </c>
+      <c r="C111" t="s">
+        <v>124</v>
+      </c>
+      <c r="D111">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B112">
+        <v>31</v>
+      </c>
+      <c r="C112" t="s">
+        <v>126</v>
+      </c>
+      <c r="D112">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B113">
+        <v>0</v>
+      </c>
+      <c r="C113" t="s">
+        <v>58</v>
+      </c>
+      <c r="D113">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B114">
+        <v>1</v>
+      </c>
+      <c r="C114" t="s">
+        <v>63</v>
+      </c>
+      <c r="D114">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="115" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B115">
+        <v>88</v>
+      </c>
+      <c r="C115" t="s">
+        <v>200</v>
+      </c>
+      <c r="D115">
+        <v>48.268517223774097</v>
+      </c>
+    </row>
+    <row r="116" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B116">
+        <v>89</v>
+      </c>
+      <c r="C116" t="s">
+        <v>201</v>
+      </c>
+      <c r="D116">
+        <v>50.840782931342297</v>
+      </c>
+    </row>
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
+      <c r="B117">
+        <v>32</v>
+      </c>
+      <c r="C117" t="s">
+        <v>128</v>
+      </c>
+      <c r="D117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B118">
+        <v>46</v>
+      </c>
+      <c r="C118" t="s">
+        <v>158</v>
+      </c>
+      <c r="D118">
+        <v>48.781019215572698</v>
+      </c>
+    </row>
+    <row r="119" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B119">
+        <v>74</v>
+      </c>
+      <c r="C119" t="s">
+        <v>186</v>
+      </c>
+      <c r="D119">
+        <v>48.781019215572698</v>
+      </c>
+    </row>
+    <row r="120" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B120">
+        <v>60</v>
+      </c>
+      <c r="C120" t="s">
+        <v>172</v>
+      </c>
+      <c r="D120">
+        <v>48.781019215572698</v>
+      </c>
+    </row>
+    <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B121">
+        <v>47</v>
+      </c>
+      <c r="C121" t="s">
+        <v>159</v>
+      </c>
+      <c r="D121">
+        <v>66.497783819115398</v>
+      </c>
+    </row>
+    <row r="122" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B122">
+        <v>75</v>
+      </c>
+      <c r="C122" t="s">
+        <v>187</v>
+      </c>
+      <c r="D122">
+        <v>66.497783819115398</v>
+      </c>
+    </row>
+    <row r="123" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
+      <c r="B123">
+        <v>61</v>
+      </c>
+      <c r="C123" t="s">
+        <v>173</v>
+      </c>
+      <c r="D123">
+        <v>66.497783819115398</v>
+      </c>
+    </row>
+  </sheetData>
+  <autoFilter ref="B1:D123" xr:uid="{2D7AFC53-E955-400B-ABBF-63B280240D92}">
+    <filterColumn colId="2">
+      <customFilters>
+        <customFilter operator="lessThan" val="40"/>
+      </customFilters>
+    </filterColumn>
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B2:D123">
+      <sortCondition ref="C1:C123"/>
+    </sortState>
+  </autoFilter>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="H1:H131">
+    <sortCondition ref="H1"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Adding files after impute
Adding files after impute
</commit_message>
<xml_diff>
--- a/helpers.xlsx
+++ b/helpers.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\AMondal2\Documents\GitHub\DataScienceCaseStudies\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Career\Upgrad\CaseStudies\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{067F55A3-46EB-4D2B-9D0B-EAD4C895726B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06AE2F83-B1B0-49E5-8F8B-4B428EEDFE4B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="9090" yWindow="195" windowWidth="14880" windowHeight="11865" activeTab="1" xr2:uid="{92DF7E96-E991-496D-91FE-46E4BCD79CFB}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="7" xr2:uid="{92DF7E96-E991-496D-91FE-46E4BCD79CFB}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,12 +20,13 @@
     <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
     <sheet name="Sheet6" sheetId="6" r:id="rId6"/>
     <sheet name="duplicate columns between dfs" sheetId="7" r:id="rId7"/>
+    <sheet name="impute" sheetId="8" r:id="rId8"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Sheet2!$A$1:$Z$163</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4" hidden="1">Sheet5!$B$1:$D$123</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,9 +34,7 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -43,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1452" uniqueCount="496">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1520" uniqueCount="564">
   <si>
     <t xml:space="preserve"> 'EMERGENCYSTATE_MODE'</t>
   </si>
@@ -1532,6 +1531,210 @@
   </si>
   <si>
     <t>Current application</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0   SK_ID_CURR                   307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1   TARGET                       307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2   NAME_CONTRACT_TYPE           307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3   CODE_GENDER                  307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4   FLAG_OWN_CAR                 307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5   FLAG_OWN_REALTY              307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6   CNT_CHILDREN                 307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7   AMT_INCOME_TOTAL             307511 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8   AMT_CREDIT                   307511 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9   AMT_ANNUITY                  307499 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10  AMT_GOODS_PRICE              307233 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11  NAME_TYPE_SUITE              306219 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12  NAME_INCOME_TYPE             307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13  NAME_EDUCATION_TYPE          307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14  NAME_FAMILY_STATUS           307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15  NAME_HOUSING_TYPE            307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16  REGION_POPULATION_RELATIVE   307511 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17  DAYS_BIRTH                   307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18  DAYS_EMPLOYED                307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19  DAYS_REGISTRATION            307511 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20  DAYS_ID_PUBLISH              307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21  OCCUPATION_TYPE              211120 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 22  CNT_FAM_MEMBERS              307509 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 23  REGION_RATING_CLIENT         307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 24  REGION_RATING_CLIENT_W_CITY  307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 25  WEEKDAY_APPR_PROCESS_START   307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 26  HOUR_APPR_PROCESS_START      307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 27  REG_REGION_NOT_LIVE_REGION   307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 28  REG_REGION_NOT_WORK_REGION   307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 29  LIVE_REGION_NOT_WORK_REGION  307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 30  REG_CITY_NOT_LIVE_CITY       307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 31  REG_CITY_NOT_WORK_CITY       307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 32  LIVE_CITY_NOT_WORK_CITY      307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 33  ORGANIZATION_TYPE            307511 non-null  category</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 34  OBS_30_CNT_SOCIAL_CIRCLE     306490 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 35  DEF_30_CNT_SOCIAL_CIRCLE     306490 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 36  OBS_60_CNT_SOCIAL_CIRCLE     306490 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 37  DEF_60_CNT_SOCIAL_CIRCLE     306490 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 38  DAYS_LAST_PHONE_CHANGE       307510 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 39  FLAG_DOCUMENT_3              307511 non-null  int64   </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 40  AMT_REQ_CREDIT_BUREAU_HOUR   265992 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 41  AMT_REQ_CREDIT_BUREAU_DAY    265992 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 42  AMT_REQ_CREDIT_BUREAU_WEEK   265992 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 43  AMT_REQ_CREDIT_BUREAU_MON    265992 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 44  AMT_REQ_CREDIT_BUREAU_QRT    265992 non-null  float64 </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 45  AMT_REQ_CREDIT_BUREAU_YEAR   265992 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 0   SK_ID_PREV              1670214 non-null  int64  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 1   SK_ID_CURR              1670214 non-null  int64  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 2   NAME_CONTRACT_TYPE      1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3   AMT_ANNUITY             1297979 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4   AMT_APPLICATION         1670214 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 5   AMT_CREDIT              1670213 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 6   AMT_GOODS_PRICE         1284699 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 7   NAME_CASH_LOAN_PURPOSE  1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 8   NAME_CONTRACT_STATUS    1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 9   DAYS_DECISION           1670214 non-null  int64  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 10  NAME_PAYMENT_TYPE       1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 11  CODE_REJECT_REASON      1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 12  NAME_CLIENT_TYPE        1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 13  NAME_GOODS_CATEGORY     1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 14  NAME_PORTFOLIO          1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 15  NAME_PRODUCT_TYPE       1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 16  CHANNEL_TYPE            1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 17  SELLERPLACE_AREA        1670214 non-null  int64  </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 18  NAME_SELLER_INDUSTRY    1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 19  CNT_PAYMENT             1297984 non-null  float64</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 20  NAME_YIELD_GROUP        1670214 non-null  object </t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 21  PRODUCT_COMBINATION     1669868 non-null  object </t>
   </si>
 </sst>
 </file>
@@ -1927,21 +2130,21 @@
       <selection activeCell="A17" sqref="A17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.42578125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="30.42578125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="31.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.453125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="31.7265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="113.45" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" ht="113.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" t="str">
         <f>CONCATENATE(E4,E5,E6,E7,E8,E9,E10,E11,E12,E13)</f>
         <v>'AMT_REQ_CREDIT_BUREAU_DAY','AMT_REQ_CREDIT_BUREAU_MON','AMT_REQ_CREDIT_BUREAU_QRT','AMT_REQ_CREDIT_BUREAU_WEEK','AMT_REQ_CREDIT_BUREAU_YEAR','EXT_SOURCE_2','EXT_SOURCE_3','HOUR_APPR_PROCESS_START','NAME_TYPE_SUITE','WEEKDAY_APPR_PROCESS_START',</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -1949,7 +2152,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -1957,7 +2160,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>31</v>
       </c>
@@ -1969,7 +2172,7 @@
         <v>'AMT_REQ_CREDIT_BUREAU_DAY',</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>17</v>
       </c>
@@ -1981,7 +2184,7 @@
         <v>'AMT_REQ_CREDIT_BUREAU_MON',</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
@@ -1993,7 +2196,7 @@
         <v>'AMT_REQ_CREDIT_BUREAU_QRT',</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>32</v>
       </c>
@@ -2005,7 +2208,7 @@
         <v>'AMT_REQ_CREDIT_BUREAU_WEEK',</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>18</v>
       </c>
@@ -2017,7 +2220,7 @@
         <v>'AMT_REQ_CREDIT_BUREAU_YEAR',</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>7</v>
       </c>
@@ -2029,7 +2232,7 @@
         <v>'EXT_SOURCE_2',</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>35</v>
       </c>
@@ -2041,7 +2244,7 @@
         <v>'EXT_SOURCE_3',</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>21</v>
       </c>
@@ -2053,7 +2256,7 @@
         <v>'HOUR_APPR_PROCESS_START',</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -2062,7 +2265,7 @@
         <v>'NAME_TYPE_SUITE',</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>36</v>
       </c>
@@ -2071,187 +2274,187 @@
         <v>'WEEKDAY_APPR_PROCESS_START',</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="17" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="18" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="19" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="20" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="21" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="22" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="23" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="24" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="25" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="26" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="27" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="28" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="29" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="30" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="31" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="32" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>44</v>
       </c>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>20</v>
       </c>
@@ -2273,20 +2476,20 @@
   <sheetPr filterMode="1"/>
   <dimension ref="A1:I163"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A129" workbookViewId="0">
+    <sheetView topLeftCell="A129" workbookViewId="0">
       <selection activeCell="C137" sqref="C137"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="21.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.28515625" style="7" customWidth="1"/>
+    <col min="2" max="2" width="21.54296875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="67.26953125" style="7" customWidth="1"/>
     <col min="5" max="5" width="49" customWidth="1"/>
-    <col min="7" max="7" width="8.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>49</v>
       </c>
@@ -2312,7 +2515,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2338,7 +2541,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2361,7 +2564,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>5</v>
       </c>
@@ -2384,7 +2587,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>6</v>
       </c>
@@ -2407,7 +2610,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>7</v>
       </c>
@@ -2430,7 +2633,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>8</v>
       </c>
@@ -2453,7 +2656,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>9</v>
       </c>
@@ -2476,7 +2679,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>10</v>
       </c>
@@ -2499,7 +2702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>11</v>
       </c>
@@ -2522,7 +2725,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>12</v>
       </c>
@@ -2545,7 +2748,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12">
         <v>13</v>
       </c>
@@ -2568,7 +2771,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13">
         <v>14</v>
       </c>
@@ -2591,7 +2794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14">
         <v>15</v>
       </c>
@@ -2614,7 +2817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15">
         <v>16</v>
       </c>
@@ -2637,7 +2840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16">
         <v>17</v>
       </c>
@@ -2660,7 +2863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17">
         <v>18</v>
       </c>
@@ -2683,7 +2886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18">
         <v>19</v>
       </c>
@@ -2709,7 +2912,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19">
         <v>20</v>
       </c>
@@ -2735,7 +2938,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20">
         <v>21</v>
       </c>
@@ -2761,7 +2964,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21">
         <v>22</v>
       </c>
@@ -2787,7 +2990,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22">
         <v>23</v>
       </c>
@@ -2813,7 +3016,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23">
         <v>24</v>
       </c>
@@ -2836,7 +3039,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24">
         <v>25</v>
       </c>
@@ -2862,7 +3065,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25">
         <v>26</v>
       </c>
@@ -2885,7 +3088,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26">
         <v>27</v>
       </c>
@@ -2908,7 +3111,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27">
         <v>28</v>
       </c>
@@ -2931,7 +3134,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28">
         <v>29</v>
       </c>
@@ -2954,7 +3157,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29">
         <v>30</v>
       </c>
@@ -2977,7 +3180,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30">
         <v>31</v>
       </c>
@@ -3000,7 +3203,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31">
         <v>32</v>
       </c>
@@ -3023,7 +3226,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32">
         <v>33</v>
       </c>
@@ -3046,7 +3249,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33">
         <v>34</v>
       </c>
@@ -3069,7 +3272,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34">
         <v>35</v>
       </c>
@@ -3092,7 +3295,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35">
         <v>36</v>
       </c>
@@ -3118,7 +3321,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36">
         <v>37</v>
       </c>
@@ -3141,7 +3344,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37">
         <v>38</v>
       </c>
@@ -3164,7 +3367,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38">
         <v>39</v>
       </c>
@@ -3187,7 +3390,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39">
         <v>40</v>
       </c>
@@ -3210,7 +3413,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40">
         <v>41</v>
       </c>
@@ -3233,7 +3436,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41">
         <v>42</v>
       </c>
@@ -3256,7 +3459,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42">
         <v>43</v>
       </c>
@@ -3279,7 +3482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43">
         <v>44</v>
       </c>
@@ -3308,7 +3511,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44">
         <v>45</v>
       </c>
@@ -3337,13 +3540,13 @@
         <v>152</v>
       </c>
     </row>
-    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
         <v>153</v>
       </c>
       <c r="D45"/>
     </row>
-    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46">
         <v>46</v>
       </c>
@@ -3369,7 +3572,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47">
         <v>47</v>
       </c>
@@ -3395,7 +3598,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48">
         <v>48</v>
       </c>
@@ -3421,7 +3624,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49">
         <v>49</v>
       </c>
@@ -3447,7 +3650,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50">
         <v>50</v>
       </c>
@@ -3473,7 +3676,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51">
         <v>51</v>
       </c>
@@ -3499,7 +3702,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52">
         <v>52</v>
       </c>
@@ -3525,7 +3728,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53">
         <v>53</v>
       </c>
@@ -3551,7 +3754,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54">
         <v>54</v>
       </c>
@@ -3577,7 +3780,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55">
         <v>55</v>
       </c>
@@ -3603,7 +3806,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56">
         <v>56</v>
       </c>
@@ -3629,7 +3832,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57">
         <v>57</v>
       </c>
@@ -3655,7 +3858,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58">
         <v>58</v>
       </c>
@@ -3681,7 +3884,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59">
         <v>59</v>
       </c>
@@ -3707,7 +3910,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60">
         <v>60</v>
       </c>
@@ -3733,7 +3936,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61">
         <v>61</v>
       </c>
@@ -3759,7 +3962,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62">
         <v>62</v>
       </c>
@@ -3785,7 +3988,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63">
         <v>63</v>
       </c>
@@ -3811,7 +4014,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64">
         <v>64</v>
       </c>
@@ -3837,7 +4040,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65">
         <v>65</v>
       </c>
@@ -3863,7 +4066,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66">
         <v>66</v>
       </c>
@@ -3889,7 +4092,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67">
         <v>67</v>
       </c>
@@ -3915,7 +4118,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68">
         <v>68</v>
       </c>
@@ -3941,7 +4144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69">
         <v>69</v>
       </c>
@@ -3967,7 +4170,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70">
         <v>70</v>
       </c>
@@ -3993,7 +4196,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71">
         <v>71</v>
       </c>
@@ -4019,7 +4222,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72">
         <v>72</v>
       </c>
@@ -4045,7 +4248,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73">
         <v>73</v>
       </c>
@@ -4071,7 +4274,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74">
         <v>74</v>
       </c>
@@ -4097,7 +4300,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75">
         <v>75</v>
       </c>
@@ -4123,7 +4326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76">
         <v>76</v>
       </c>
@@ -4149,7 +4352,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77">
         <v>77</v>
       </c>
@@ -4175,7 +4378,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78">
         <v>78</v>
       </c>
@@ -4201,7 +4404,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79">
         <v>79</v>
       </c>
@@ -4227,7 +4430,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80">
         <v>80</v>
       </c>
@@ -4253,7 +4456,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81">
         <v>81</v>
       </c>
@@ -4279,7 +4482,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82">
         <v>82</v>
       </c>
@@ -4305,7 +4508,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83">
         <v>83</v>
       </c>
@@ -4331,7 +4534,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84">
         <v>84</v>
       </c>
@@ -4357,7 +4560,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85">
         <v>85</v>
       </c>
@@ -4383,7 +4586,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86">
         <v>86</v>
       </c>
@@ -4409,7 +4612,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87">
         <v>87</v>
       </c>
@@ -4435,7 +4638,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88">
         <v>88</v>
       </c>
@@ -4461,7 +4664,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89">
         <v>89</v>
       </c>
@@ -4487,7 +4690,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90">
         <v>90</v>
       </c>
@@ -4513,7 +4716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91">
         <v>91</v>
       </c>
@@ -4539,7 +4742,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92">
         <v>92</v>
       </c>
@@ -4565,7 +4768,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93">
         <v>93</v>
       </c>
@@ -4591,7 +4794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94">
         <v>94</v>
       </c>
@@ -4614,7 +4817,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95">
         <v>95</v>
       </c>
@@ -4637,7 +4840,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96">
         <v>96</v>
       </c>
@@ -4660,7 +4863,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97">
         <v>97</v>
       </c>
@@ -4683,7 +4886,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98">
         <v>98</v>
       </c>
@@ -4709,7 +4912,7 @@
         <v>213</v>
       </c>
     </row>
-    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99">
         <v>99</v>
       </c>
@@ -4732,7 +4935,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100">
         <v>100</v>
       </c>
@@ -4755,7 +4958,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101">
         <v>101</v>
       </c>
@@ -4778,7 +4981,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102">
         <v>102</v>
       </c>
@@ -4801,7 +5004,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103">
         <v>103</v>
       </c>
@@ -4824,7 +5027,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104">
         <v>104</v>
       </c>
@@ -4847,7 +5050,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105">
         <v>105</v>
       </c>
@@ -4870,7 +5073,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106">
         <v>106</v>
       </c>
@@ -4893,7 +5096,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107">
         <v>107</v>
       </c>
@@ -4916,7 +5119,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108">
         <v>108</v>
       </c>
@@ -4939,7 +5142,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109">
         <v>109</v>
       </c>
@@ -4962,7 +5165,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110">
         <v>110</v>
       </c>
@@ -4985,7 +5188,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111">
         <v>111</v>
       </c>
@@ -5008,7 +5211,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112">
         <v>112</v>
       </c>
@@ -5031,7 +5234,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113">
         <v>113</v>
       </c>
@@ -5054,7 +5257,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114">
         <v>114</v>
       </c>
@@ -5077,7 +5280,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>115</v>
       </c>
@@ -5100,7 +5303,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>116</v>
       </c>
@@ -5123,7 +5326,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>117</v>
       </c>
@@ -5146,7 +5349,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>118</v>
       </c>
@@ -5169,7 +5372,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>119</v>
       </c>
@@ -5195,13 +5398,13 @@
         <v>256</v>
       </c>
     </row>
-    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120" t="s">
         <v>257</v>
       </c>
       <c r="D120"/>
     </row>
-    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>120</v>
       </c>
@@ -5224,7 +5427,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>121</v>
       </c>
@@ -5247,7 +5450,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>122</v>
       </c>
@@ -5270,7 +5473,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>123</v>
       </c>
@@ -5293,7 +5496,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>124</v>
       </c>
@@ -5316,7 +5519,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="126" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>176</v>
       </c>
@@ -5345,7 +5548,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>177</v>
       </c>
@@ -5371,7 +5574,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>178</v>
       </c>
@@ -5394,7 +5597,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>179</v>
       </c>
@@ -5417,7 +5620,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>180</v>
       </c>
@@ -5440,7 +5643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="131" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:9" ht="58" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>181</v>
       </c>
@@ -5463,7 +5666,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="132" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>182</v>
       </c>
@@ -5486,7 +5689,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="133" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>183</v>
       </c>
@@ -5512,7 +5715,7 @@
         <v>281</v>
       </c>
     </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>184</v>
       </c>
@@ -5535,7 +5738,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="135" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>185</v>
       </c>
@@ -5561,7 +5764,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="136" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A136">
         <v>186</v>
       </c>
@@ -5584,7 +5787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:9" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A137">
         <v>187</v>
       </c>
@@ -5607,7 +5810,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A138">
         <v>188</v>
       </c>
@@ -5630,7 +5833,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A139">
         <v>189</v>
       </c>
@@ -5656,7 +5859,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A140">
         <v>190</v>
       </c>
@@ -5682,7 +5885,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A141">
         <v>191</v>
       </c>
@@ -5708,7 +5911,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A142">
         <v>192</v>
       </c>
@@ -5731,7 +5934,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A143">
         <v>193</v>
       </c>
@@ -5754,7 +5957,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="144" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A144">
         <v>194</v>
       </c>
@@ -5780,7 +5983,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="145" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A145">
         <v>195</v>
       </c>
@@ -5803,7 +6006,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A146">
         <v>196</v>
       </c>
@@ -5826,7 +6029,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A147">
         <v>197</v>
       </c>
@@ -5849,7 +6052,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="148" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A148">
         <v>198</v>
       </c>
@@ -5872,7 +6075,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="149" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A149">
         <v>199</v>
       </c>
@@ -5895,7 +6098,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="150" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A150">
         <v>200</v>
       </c>
@@ -5918,7 +6121,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="151" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A151">
         <v>201</v>
       </c>
@@ -5941,7 +6144,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="152" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A152">
         <v>202</v>
       </c>
@@ -5964,7 +6167,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="153" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A153">
         <v>203</v>
       </c>
@@ -5987,7 +6190,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="154" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A154">
         <v>204</v>
       </c>
@@ -6010,7 +6213,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="155" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A155">
         <v>205</v>
       </c>
@@ -6033,7 +6236,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="156" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A156">
         <v>206</v>
       </c>
@@ -6059,7 +6262,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="157" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A157">
         <v>207</v>
       </c>
@@ -6082,7 +6285,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="158" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A158">
         <v>208</v>
       </c>
@@ -6108,7 +6311,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="159" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A159">
         <v>209</v>
       </c>
@@ -6134,7 +6337,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="160" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A160">
         <v>210</v>
       </c>
@@ -6160,7 +6363,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="161" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A161">
         <v>211</v>
       </c>
@@ -6186,7 +6389,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="162" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:8" ht="29" x14ac:dyDescent="0.35">
       <c r="A162">
         <v>212</v>
       </c>
@@ -6212,7 +6415,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A163">
         <v>213</v>
       </c>
@@ -6259,12 +6462,12 @@
       <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="55.28515625" customWidth="1"/>
+    <col min="2" max="2" width="55.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="5" spans="2:2" ht="156.94999999999999" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:2" ht="157" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B5" s="3" t="s">
         <v>339</v>
       </c>
@@ -6286,22 +6489,22 @@
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="65.28515625" customWidth="1"/>
+    <col min="1" max="1" width="65.26953125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" ht="160.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" ht="160.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>340</v>
       </c>
     </row>
-    <row r="2" spans="1:1" ht="258.95" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" ht="259" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5" t="s">
         <v>343</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" s="1"/>
     </row>
   </sheetData>
@@ -6322,15 +6525,15 @@
       <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="31.5703125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="30.7109375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="33.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="31.54296875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="30.7265625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="33.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:8" x14ac:dyDescent="0.35">
       <c r="C1" t="s">
         <v>341</v>
       </c>
@@ -6347,7 +6550,7 @@
         <v>346</v>
       </c>
     </row>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>9</v>
       </c>
@@ -6367,7 +6570,7 @@
         <v>360</v>
       </c>
     </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B3">
         <v>8</v>
       </c>
@@ -6387,7 +6590,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B4">
         <v>10</v>
       </c>
@@ -6407,7 +6610,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5">
         <v>7</v>
       </c>
@@ -6427,7 +6630,7 @@
         <v>350</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6">
         <v>117</v>
       </c>
@@ -6447,7 +6650,7 @@
         <v>351</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7">
         <v>116</v>
       </c>
@@ -6467,7 +6670,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8">
         <v>119</v>
       </c>
@@ -6487,7 +6690,7 @@
         <v>352</v>
       </c>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B9">
         <v>120</v>
       </c>
@@ -6507,7 +6710,7 @@
         <v>366</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10">
         <v>118</v>
       </c>
@@ -6527,7 +6730,7 @@
         <v>345</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11">
         <v>121</v>
       </c>
@@ -6547,7 +6750,7 @@
         <v>353</v>
       </c>
     </row>
-    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B12">
         <v>44</v>
       </c>
@@ -6567,7 +6770,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B13">
         <v>72</v>
       </c>
@@ -6587,7 +6790,7 @@
         <v>355</v>
       </c>
     </row>
-    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B14">
         <v>58</v>
       </c>
@@ -6607,7 +6810,7 @@
         <v>356</v>
       </c>
     </row>
-    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B15">
         <v>45</v>
       </c>
@@ -6627,7 +6830,7 @@
         <v>357</v>
       </c>
     </row>
-    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B16">
         <v>73</v>
       </c>
@@ -6647,7 +6850,7 @@
         <v>358</v>
       </c>
     </row>
-    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B17">
         <v>59</v>
       </c>
@@ -6667,7 +6870,7 @@
         <v>359</v>
       </c>
     </row>
-    <row r="18" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B18">
         <v>6</v>
       </c>
@@ -6687,7 +6890,7 @@
         <v>381</v>
       </c>
     </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B19">
         <v>29</v>
       </c>
@@ -6707,7 +6910,7 @@
         <v>367</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B20">
         <v>3</v>
       </c>
@@ -6727,7 +6930,7 @@
         <v>382</v>
       </c>
     </row>
-    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B21">
         <v>48</v>
       </c>
@@ -6747,7 +6950,7 @@
         <v>363</v>
       </c>
     </row>
-    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B22">
         <v>76</v>
       </c>
@@ -6767,7 +6970,7 @@
         <v>364</v>
       </c>
     </row>
-    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B23">
         <v>62</v>
       </c>
@@ -6787,7 +6990,7 @@
         <v>365</v>
       </c>
     </row>
-    <row r="24" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B24">
         <v>17</v>
       </c>
@@ -6807,7 +7010,7 @@
         <v>368</v>
       </c>
     </row>
-    <row r="25" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25">
         <v>18</v>
       </c>
@@ -6827,7 +7030,7 @@
         <v>388</v>
       </c>
     </row>
-    <row r="26" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26">
         <v>20</v>
       </c>
@@ -6847,7 +7050,7 @@
         <v>389</v>
       </c>
     </row>
-    <row r="27" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27">
         <v>95</v>
       </c>
@@ -6867,7 +7070,7 @@
         <v>383</v>
       </c>
     </row>
-    <row r="28" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28">
         <v>19</v>
       </c>
@@ -6887,7 +7090,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="29" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29">
         <v>92</v>
       </c>
@@ -6907,7 +7110,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="30" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B30">
         <v>94</v>
       </c>
@@ -6927,7 +7130,7 @@
         <v>370</v>
       </c>
     </row>
-    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B31">
         <v>49</v>
       </c>
@@ -6947,7 +7150,7 @@
         <v>373</v>
       </c>
     </row>
-    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B32">
         <v>77</v>
       </c>
@@ -6967,7 +7170,7 @@
         <v>374</v>
       </c>
     </row>
-    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B33">
         <v>63</v>
       </c>
@@ -6987,7 +7190,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B34">
         <v>90</v>
       </c>
@@ -7007,7 +7210,7 @@
         <v>376</v>
       </c>
     </row>
-    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B35">
         <v>50</v>
       </c>
@@ -7027,7 +7230,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B36">
         <v>78</v>
       </c>
@@ -7047,7 +7250,7 @@
         <v>378</v>
       </c>
     </row>
-    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B37">
         <v>64</v>
       </c>
@@ -7067,7 +7270,7 @@
         <v>379</v>
       </c>
     </row>
-    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="B38">
         <v>41</v>
       </c>
@@ -7087,7 +7290,7 @@
         <v>380</v>
       </c>
     </row>
-    <row r="39" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B39">
         <v>42</v>
       </c>
@@ -7107,7 +7310,7 @@
         <v>385</v>
       </c>
     </row>
-    <row r="40" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B40">
         <v>43</v>
       </c>
@@ -7127,7 +7330,7 @@
         <v>371</v>
       </c>
     </row>
-    <row r="41" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B41">
         <v>25</v>
       </c>
@@ -7147,7 +7350,7 @@
         <v>386</v>
       </c>
     </row>
-    <row r="42" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B42">
         <v>104</v>
       </c>
@@ -7167,7 +7370,7 @@
         <v>372</v>
       </c>
     </row>
-    <row r="43" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B43">
         <v>105</v>
       </c>
@@ -7187,7 +7390,7 @@
         <v>387</v>
       </c>
     </row>
-    <row r="44" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B44">
         <v>106</v>
       </c>
@@ -7207,7 +7410,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="45" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B45">
         <v>107</v>
       </c>
@@ -7227,7 +7430,7 @@
         <v>391</v>
       </c>
     </row>
-    <row r="46" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B46">
         <v>108</v>
       </c>
@@ -7247,7 +7450,7 @@
         <v>348</v>
       </c>
     </row>
-    <row r="47" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B47">
         <v>109</v>
       </c>
@@ -7267,7 +7470,7 @@
         <v>362</v>
       </c>
     </row>
-    <row r="48" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B48">
         <v>110</v>
       </c>
@@ -7287,7 +7490,7 @@
         <v>349</v>
       </c>
     </row>
-    <row r="49" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="49" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B49">
         <v>111</v>
       </c>
@@ -7307,7 +7510,7 @@
         <v>344</v>
       </c>
     </row>
-    <row r="50" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B50">
         <v>112</v>
       </c>
@@ -7324,7 +7527,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="51" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B51">
         <v>113</v>
       </c>
@@ -7341,7 +7544,7 @@
         <v>228</v>
       </c>
     </row>
-    <row r="52" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B52">
         <v>96</v>
       </c>
@@ -7358,7 +7561,7 @@
         <v>118</v>
       </c>
     </row>
-    <row r="53" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B53">
         <v>114</v>
       </c>
@@ -7375,7 +7578,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="54" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B54">
         <v>115</v>
       </c>
@@ -7392,7 +7595,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="55" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="55" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B55">
         <v>97</v>
       </c>
@@ -7409,7 +7612,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="56" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B56">
         <v>98</v>
       </c>
@@ -7426,7 +7629,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="57" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B57">
         <v>99</v>
       </c>
@@ -7443,7 +7646,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="58" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B58">
         <v>100</v>
       </c>
@@ -7460,7 +7663,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="59" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B59">
         <v>101</v>
       </c>
@@ -7477,7 +7680,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="60" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B60">
         <v>102</v>
       </c>
@@ -7494,7 +7697,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="61" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B61">
         <v>103</v>
       </c>
@@ -7511,7 +7714,7 @@
         <v>207</v>
       </c>
     </row>
-    <row r="62" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B62">
         <v>27</v>
       </c>
@@ -7528,7 +7731,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="63" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B63">
         <v>23</v>
       </c>
@@ -7545,7 +7748,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="64" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B64">
         <v>22</v>
       </c>
@@ -7562,7 +7765,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="65" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B65">
         <v>4</v>
       </c>
@@ -7579,7 +7782,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="66" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B66">
         <v>5</v>
       </c>
@@ -7596,7 +7799,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="67" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B67">
         <v>26</v>
       </c>
@@ -7613,7 +7816,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="68" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B68">
         <v>24</v>
       </c>
@@ -7624,7 +7827,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="69" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B69">
         <v>51</v>
       </c>
@@ -7641,7 +7844,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="70" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B70">
         <v>79</v>
       </c>
@@ -7658,7 +7861,7 @@
         <v>258</v>
       </c>
     </row>
-    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B71">
         <v>65</v>
       </c>
@@ -7675,7 +7878,7 @@
         <v>260</v>
       </c>
     </row>
-    <row r="72" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B72">
         <v>52</v>
       </c>
@@ -7692,7 +7895,7 @@
         <v>262</v>
       </c>
     </row>
-    <row r="73" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B73">
         <v>80</v>
       </c>
@@ -7709,7 +7912,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="74" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B74">
         <v>66</v>
       </c>
@@ -7726,7 +7929,7 @@
         <v>266</v>
       </c>
     </row>
-    <row r="75" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B75">
         <v>86</v>
       </c>
@@ -7737,7 +7940,7 @@
         <v>68.386171551586699</v>
       </c>
     </row>
-    <row r="76" spans="2:7" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:7" x14ac:dyDescent="0.35">
       <c r="B76">
         <v>33</v>
       </c>
@@ -7748,7 +7951,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="77" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B77">
         <v>87</v>
       </c>
@@ -7759,7 +7962,7 @@
         <v>50.176091261776001</v>
       </c>
     </row>
-    <row r="78" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B78">
         <v>53</v>
       </c>
@@ -7770,7 +7973,7 @@
         <v>59.376737742714802</v>
       </c>
     </row>
-    <row r="79" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B79">
         <v>81</v>
       </c>
@@ -7781,7 +7984,7 @@
         <v>59.376737742714802</v>
       </c>
     </row>
-    <row r="80" spans="2:7" hidden="1" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:7" hidden="1" x14ac:dyDescent="0.35">
       <c r="B80">
         <v>67</v>
       </c>
@@ -7792,7 +7995,7 @@
         <v>59.376737742714802</v>
       </c>
     </row>
-    <row r="81" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B81">
         <v>39</v>
       </c>
@@ -7803,7 +8006,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="82" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B82">
         <v>36</v>
       </c>
@@ -7814,7 +8017,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="83" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B83">
         <v>54</v>
       </c>
@@ -7825,7 +8028,7 @@
         <v>68.354953156147204</v>
       </c>
     </row>
-    <row r="84" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B84">
         <v>82</v>
       </c>
@@ -7836,7 +8039,7 @@
         <v>68.354953156147204</v>
       </c>
     </row>
-    <row r="85" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B85">
         <v>68</v>
       </c>
@@ -7847,7 +8050,7 @@
         <v>68.354953156147204</v>
       </c>
     </row>
-    <row r="86" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B86">
         <v>55</v>
       </c>
@@ -7858,7 +8061,7 @@
         <v>50.1933264175915</v>
       </c>
     </row>
-    <row r="87" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B87">
         <v>83</v>
       </c>
@@ -7869,7 +8072,7 @@
         <v>50.1933264175915</v>
       </c>
     </row>
-    <row r="88" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B88">
         <v>69</v>
       </c>
@@ -7880,7 +8083,7 @@
         <v>50.1933264175915</v>
       </c>
     </row>
-    <row r="89" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B89">
         <v>2</v>
       </c>
@@ -7891,7 +8094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B90">
         <v>13</v>
       </c>
@@ -7902,7 +8105,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B91">
         <v>14</v>
       </c>
@@ -7913,7 +8116,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="92" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B92">
         <v>15</v>
       </c>
@@ -7924,7 +8127,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="93" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B93">
         <v>12</v>
       </c>
@@ -7935,7 +8138,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="94" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B94">
         <v>11</v>
       </c>
@@ -7946,7 +8149,7 @@
         <v>0.42014757195677499</v>
       </c>
     </row>
-    <row r="95" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B95">
         <v>56</v>
       </c>
@@ -7957,7 +8160,7 @@
         <v>69.432963373667903</v>
       </c>
     </row>
-    <row r="96" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B96">
         <v>84</v>
       </c>
@@ -7968,7 +8171,7 @@
         <v>69.432963373667903</v>
       </c>
     </row>
-    <row r="97" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="97" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B97">
         <v>70</v>
       </c>
@@ -7979,7 +8182,7 @@
         <v>69.432963373667903</v>
       </c>
     </row>
-    <row r="98" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="98" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B98">
         <v>57</v>
       </c>
@@ -7990,7 +8193,7 @@
         <v>55.179164322577002</v>
       </c>
     </row>
-    <row r="99" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="99" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B99">
         <v>85</v>
       </c>
@@ -8001,7 +8204,7 @@
         <v>55.179164322577002</v>
       </c>
     </row>
-    <row r="100" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="100" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B100">
         <v>71</v>
       </c>
@@ -8012,7 +8215,7 @@
         <v>55.179164322577002</v>
       </c>
     </row>
-    <row r="101" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="101" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B101">
         <v>91</v>
       </c>
@@ -8023,7 +8226,7 @@
         <v>0.332020643163984</v>
       </c>
     </row>
-    <row r="102" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="102" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B102">
         <v>93</v>
       </c>
@@ -8034,7 +8237,7 @@
         <v>0.332020643163984</v>
       </c>
     </row>
-    <row r="103" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="103" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B103">
         <v>28</v>
       </c>
@@ -8045,7 +8248,7 @@
         <v>31.345545362604899</v>
       </c>
     </row>
-    <row r="104" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="104" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B104">
         <v>40</v>
       </c>
@@ -8056,7 +8259,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="105" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="105" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B105">
         <v>21</v>
       </c>
@@ -8067,7 +8270,7 @@
         <v>65.990810084842494</v>
       </c>
     </row>
-    <row r="106" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="106" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B106">
         <v>37</v>
       </c>
@@ -8078,7 +8281,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="107" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="107" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B107">
         <v>38</v>
       </c>
@@ -8089,7 +8292,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="108" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="108" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B108">
         <v>34</v>
       </c>
@@ -8100,7 +8303,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="109" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="109" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B109">
         <v>35</v>
       </c>
@@ -8111,7 +8314,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="110" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B110">
         <v>16</v>
       </c>
@@ -8122,7 +8325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="111" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B111">
         <v>30</v>
       </c>
@@ -8133,7 +8336,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="112" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B112">
         <v>31</v>
       </c>
@@ -8144,7 +8347,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B113">
         <v>0</v>
       </c>
@@ -8155,7 +8358,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B114">
         <v>1</v>
       </c>
@@ -8166,7 +8369,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B115">
         <v>88</v>
       </c>
@@ -8177,7 +8380,7 @@
         <v>48.268517223774097</v>
       </c>
     </row>
-    <row r="116" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B116">
         <v>89</v>
       </c>
@@ -8188,7 +8391,7 @@
         <v>50.840782931342297</v>
       </c>
     </row>
-    <row r="117" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B117">
         <v>32</v>
       </c>
@@ -8199,7 +8402,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="118" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="118" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B118">
         <v>46</v>
       </c>
@@ -8210,7 +8413,7 @@
         <v>48.781019215572698</v>
       </c>
     </row>
-    <row r="119" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="119" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B119">
         <v>74</v>
       </c>
@@ -8221,7 +8424,7 @@
         <v>48.781019215572698</v>
       </c>
     </row>
-    <row r="120" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B120">
         <v>60</v>
       </c>
@@ -8232,7 +8435,7 @@
         <v>48.781019215572698</v>
       </c>
     </row>
-    <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B121">
         <v>47</v>
       </c>
@@ -8243,7 +8446,7 @@
         <v>66.497783819115398</v>
       </c>
     </row>
-    <row r="122" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B122">
         <v>75</v>
       </c>
@@ -8254,7 +8457,7 @@
         <v>66.497783819115398</v>
       </c>
     </row>
-    <row r="123" spans="2:4" hidden="1" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:4" hidden="1" x14ac:dyDescent="0.35">
       <c r="B123">
         <v>61</v>
       </c>
@@ -8295,14 +8498,14 @@
       <selection activeCell="A51" sqref="A51"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="26.140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.1796875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="26.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>495</v>
       </c>
@@ -8313,7 +8516,7 @@
         <v>485</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>480</v>
       </c>
@@ -8324,7 +8527,7 @@
         <v>401</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>479</v>
       </c>
@@ -8335,7 +8538,7 @@
         <v>457</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>481</v>
       </c>
@@ -8346,7 +8549,7 @@
         <v>458</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>399</v>
       </c>
@@ -8357,7 +8560,7 @@
         <v>400</v>
       </c>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>482</v>
       </c>
@@ -8368,7 +8571,7 @@
         <v>459</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>398</v>
       </c>
@@ -8379,7 +8582,7 @@
         <v>402</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>419</v>
       </c>
@@ -8390,7 +8593,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>395</v>
       </c>
@@ -8401,7 +8604,7 @@
         <v>399</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>408</v>
       </c>
@@ -8412,7 +8615,7 @@
         <v>454</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>409</v>
       </c>
@@ -8423,7 +8626,7 @@
         <v>472</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>411</v>
       </c>
@@ -8434,7 +8637,7 @@
         <v>398</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>433</v>
       </c>
@@ -8445,7 +8648,7 @@
         <v>419</v>
       </c>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>410</v>
       </c>
@@ -8456,7 +8659,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>430</v>
       </c>
@@ -8467,7 +8670,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>432</v>
       </c>
@@ -8478,7 +8681,7 @@
         <v>467</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>415</v>
       </c>
@@ -8489,7 +8692,7 @@
         <v>408</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>442</v>
       </c>
@@ -8500,7 +8703,7 @@
         <v>465</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>443</v>
       </c>
@@ -8511,7 +8714,7 @@
         <v>409</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>444</v>
       </c>
@@ -8522,7 +8725,7 @@
         <v>411</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>445</v>
       </c>
@@ -8533,7 +8736,7 @@
         <v>433</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>446</v>
       </c>
@@ -8544,7 +8747,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>447</v>
       </c>
@@ -8555,7 +8758,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>448</v>
       </c>
@@ -8566,7 +8769,7 @@
         <v>432</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>449</v>
       </c>
@@ -8577,7 +8780,7 @@
         <v>415</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>450</v>
       </c>
@@ -8585,7 +8788,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>451</v>
       </c>
@@ -8593,7 +8796,7 @@
         <v>443</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>434</v>
       </c>
@@ -8601,7 +8804,7 @@
         <v>444</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>452</v>
       </c>
@@ -8609,7 +8812,7 @@
         <v>445</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>453</v>
       </c>
@@ -8617,7 +8820,7 @@
         <v>446</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>435</v>
       </c>
@@ -8625,7 +8828,7 @@
         <v>447</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>436</v>
       </c>
@@ -8633,7 +8836,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>437</v>
       </c>
@@ -8641,7 +8844,7 @@
         <v>449</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>438</v>
       </c>
@@ -8649,7 +8852,7 @@
         <v>450</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>439</v>
       </c>
@@ -8657,7 +8860,7 @@
         <v>451</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>440</v>
       </c>
@@ -8665,7 +8868,7 @@
         <v>434</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>441</v>
       </c>
@@ -8673,7 +8876,7 @@
         <v>452</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>417</v>
       </c>
@@ -8681,7 +8884,7 @@
         <v>453</v>
       </c>
     </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>413</v>
       </c>
@@ -8689,7 +8892,7 @@
         <v>435</v>
       </c>
     </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>412</v>
       </c>
@@ -8697,7 +8900,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>396</v>
       </c>
@@ -8705,7 +8908,7 @@
         <v>437</v>
       </c>
     </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>397</v>
       </c>
@@ -8713,7 +8916,7 @@
         <v>438</v>
       </c>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>416</v>
       </c>
@@ -8721,7 +8924,7 @@
         <v>439</v>
       </c>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>414</v>
       </c>
@@ -8729,7 +8932,7 @@
         <v>440</v>
       </c>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>427</v>
       </c>
@@ -8737,7 +8940,7 @@
         <v>441</v>
       </c>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>424</v>
       </c>
@@ -8745,7 +8948,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>478</v>
       </c>
@@ -8753,7 +8956,7 @@
         <v>413</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>404</v>
       </c>
@@ -8761,7 +8964,7 @@
         <v>461</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>405</v>
       </c>
@@ -8769,7 +8972,7 @@
         <v>412</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>406</v>
       </c>
@@ -8777,7 +8980,7 @@
         <v>396</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>403</v>
       </c>
@@ -8785,7 +8988,7 @@
         <v>397</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>429</v>
       </c>
@@ -8793,7 +8996,7 @@
         <v>416</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>431</v>
       </c>
@@ -8801,7 +9004,7 @@
         <v>414</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>418</v>
       </c>
@@ -8809,7 +9012,7 @@
         <v>427</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>428</v>
       </c>
@@ -8817,7 +9020,7 @@
         <v>424</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>425</v>
       </c>
@@ -8825,7 +9028,7 @@
         <v>463</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>426</v>
       </c>
@@ -8833,7 +9036,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>422</v>
       </c>
@@ -8841,7 +9044,7 @@
         <v>464</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>423</v>
       </c>
@@ -8849,7 +9052,7 @@
         <v>394</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>407</v>
       </c>
@@ -8857,7 +9060,7 @@
         <v>456</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>420</v>
       </c>
@@ -8865,7 +9068,7 @@
         <v>404</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>421</v>
       </c>
@@ -8873,7 +9076,7 @@
         <v>405</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>393</v>
       </c>
@@ -8881,7 +9084,7 @@
         <v>469</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>392</v>
       </c>
@@ -8889,117 +9092,117 @@
         <v>406</v>
       </c>
     </row>
-    <row r="65" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="65" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E65" s="1" t="s">
         <v>403</v>
       </c>
     </row>
-    <row r="66" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="66" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E66" s="1" t="s">
         <v>466</v>
       </c>
     </row>
-    <row r="67" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="67" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E67" s="1" t="s">
         <v>470</v>
       </c>
     </row>
-    <row r="68" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="68" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E68" s="1" t="s">
         <v>471</v>
       </c>
     </row>
-    <row r="69" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="69" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E69" s="1" t="s">
         <v>474</v>
       </c>
     </row>
-    <row r="70" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="70" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E70" s="1" t="s">
         <v>476</v>
       </c>
     </row>
-    <row r="71" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="71" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E71" s="1" t="s">
         <v>462</v>
       </c>
     </row>
-    <row r="72" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="72" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E72" s="1" t="s">
         <v>429</v>
       </c>
     </row>
-    <row r="73" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="73" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E73" s="1" t="s">
         <v>431</v>
       </c>
     </row>
-    <row r="74" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="74" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E74" s="1" t="s">
         <v>418</v>
       </c>
     </row>
-    <row r="75" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="75" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E75" s="1" t="s">
         <v>428</v>
       </c>
     </row>
-    <row r="76" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="76" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E76" s="1" t="s">
         <v>477</v>
       </c>
     </row>
-    <row r="77" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="77" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E77" s="1" t="s">
         <v>425</v>
       </c>
     </row>
-    <row r="78" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="78" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E78" s="1" t="s">
         <v>426</v>
       </c>
     </row>
-    <row r="79" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="79" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E79" s="1" t="s">
         <v>422</v>
       </c>
     </row>
-    <row r="80" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="80" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E80" s="1" t="s">
         <v>423</v>
       </c>
     </row>
-    <row r="81" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="81" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E81" s="1" t="s">
         <v>407</v>
       </c>
     </row>
-    <row r="82" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="82" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E82" s="1" t="s">
         <v>420</v>
       </c>
     </row>
-    <row r="83" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="83" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E83" s="1" t="s">
         <v>421</v>
       </c>
     </row>
-    <row r="84" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="84" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E84" s="1" t="s">
         <v>473</v>
       </c>
     </row>
-    <row r="85" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="85" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E85" s="1" t="s">
         <v>455</v>
       </c>
     </row>
-    <row r="86" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="86" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E86" s="1" t="s">
         <v>393</v>
       </c>
     </row>
-    <row r="87" spans="5:5" x14ac:dyDescent="0.25">
+    <row r="87" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E87" s="1" t="s">
         <v>392</v>
       </c>
@@ -9024,47 +9227,47 @@
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="23.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>486</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
         <v>487</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>488</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>489</v>
       </c>
     </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>490</v>
       </c>
     </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
         <v>491</v>
       </c>
     </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>492</v>
       </c>
     </row>
-    <row r="8" spans="1:1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:1" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>493</v>
       </c>
@@ -9079,4 +9282,320 @@
     <oddFooter>&amp;C&amp;1#&amp;"Calibri"&amp;10&amp;K000000Schlumberger-Private</oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3F6087D-7D41-4FC8-8430-59D4C5D0C9F8}">
+  <dimension ref="A1:E46"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D5" sqref="D5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="44.26953125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="40.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>496</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>542</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A2" s="1" t="s">
+        <v>497</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>543</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A3" s="1" t="s">
+        <v>498</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>544</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A4" s="1" t="s">
+        <v>499</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>545</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>500</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>546</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A6" s="1" t="s">
+        <v>501</v>
+      </c>
+      <c r="E6" s="1" t="s">
+        <v>547</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A7" s="1" t="s">
+        <v>502</v>
+      </c>
+      <c r="E7" s="1" t="s">
+        <v>548</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A8" s="1" t="s">
+        <v>503</v>
+      </c>
+      <c r="E8" s="1" t="s">
+        <v>549</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A9" s="1" t="s">
+        <v>504</v>
+      </c>
+      <c r="E9" s="1" t="s">
+        <v>550</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A10" s="1" t="s">
+        <v>505</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>551</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A11" s="1" t="s">
+        <v>506</v>
+      </c>
+      <c r="E11" s="1" t="s">
+        <v>552</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A12" s="1" t="s">
+        <v>507</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>553</v>
+      </c>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A13" s="1" t="s">
+        <v>508</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>554</v>
+      </c>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A14" s="1" t="s">
+        <v>509</v>
+      </c>
+      <c r="E14" s="1" t="s">
+        <v>555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A15" s="1" t="s">
+        <v>510</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>556</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A16" s="1" t="s">
+        <v>511</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>557</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A17" s="1" t="s">
+        <v>512</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>558</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A18" s="1" t="s">
+        <v>513</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>559</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A19" s="1" t="s">
+        <v>514</v>
+      </c>
+      <c r="E19" s="1" t="s">
+        <v>560</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A20" s="1" t="s">
+        <v>515</v>
+      </c>
+      <c r="E20" s="1" t="s">
+        <v>561</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A21" s="1" t="s">
+        <v>516</v>
+      </c>
+      <c r="E21" s="1" t="s">
+        <v>562</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A22" s="1" t="s">
+        <v>517</v>
+      </c>
+      <c r="E22" s="1" t="s">
+        <v>563</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A23" s="1" t="s">
+        <v>518</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A24" s="1" t="s">
+        <v>519</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A25" s="1" t="s">
+        <v>520</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A26" s="1" t="s">
+        <v>521</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A27" s="1" t="s">
+        <v>522</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A28" s="1" t="s">
+        <v>523</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A29" s="1" t="s">
+        <v>524</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A30" s="1" t="s">
+        <v>525</v>
+      </c>
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A31" s="1" t="s">
+        <v>526</v>
+      </c>
+    </row>
+    <row r="32" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A32" s="1" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="33" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A33" s="1" t="s">
+        <v>528</v>
+      </c>
+    </row>
+    <row r="34" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A34" s="1" t="s">
+        <v>529</v>
+      </c>
+    </row>
+    <row r="35" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A35" s="1" t="s">
+        <v>530</v>
+      </c>
+    </row>
+    <row r="36" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A36" s="1" t="s">
+        <v>531</v>
+      </c>
+    </row>
+    <row r="37" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A37" s="1" t="s">
+        <v>532</v>
+      </c>
+    </row>
+    <row r="38" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A38" s="1" t="s">
+        <v>533</v>
+      </c>
+    </row>
+    <row r="39" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A39" s="1" t="s">
+        <v>534</v>
+      </c>
+    </row>
+    <row r="40" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A40" s="1" t="s">
+        <v>535</v>
+      </c>
+    </row>
+    <row r="41" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A41" s="1" t="s">
+        <v>536</v>
+      </c>
+    </row>
+    <row r="42" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A42" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+    <row r="43" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A43" s="1" t="s">
+        <v>538</v>
+      </c>
+    </row>
+    <row r="44" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A44" s="1" t="s">
+        <v>539</v>
+      </c>
+    </row>
+    <row r="45" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A45" s="1" t="s">
+        <v>540</v>
+      </c>
+    </row>
+    <row r="46" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A46" s="1" t="s">
+        <v>541</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>